<commit_message>
git commit 27th feb
</commit_message>
<xml_diff>
--- a/src/Arrays/ArrayUtility.xlsx
+++ b/src/Arrays/ArrayUtility.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niteshkumar/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niteshkumar/IdeaProjects/DS_Java/src/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D51215-37CC-6346-9E3B-17858228AFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC74139F-587B-184F-B0E1-4AFC0F963461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="780" windowWidth="19760" windowHeight="16940" activeTab="1" xr2:uid="{817E162C-D097-FF46-BB32-EACBC3A386A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{817E162C-D097-FF46-BB32-EACBC3A386A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="clone" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
   <si>
     <t>Method Name</t>
   </si>
@@ -402,6 +403,171 @@
       </rPr>
       <t> are compared to each other.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Int </t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Int []</t>
+  </si>
+  <si>
+    <t>String []</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in copy </t>
+  </si>
+  <si>
+    <t>Mutable</t>
+  </si>
+  <si>
+    <t>Immutable</t>
+  </si>
+  <si>
+    <t>&lt;Mutable&gt;</t>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+  </si>
+  <si>
+    <t>["hi","bye"]</t>
+  </si>
+  <si>
+    <t>"hi"</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Clone</t>
+  </si>
+  <si>
+    <t>int[].clone()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applying clone on object - deep copy will get created </t>
+  </si>
+  <si>
+    <t>deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shallow </t>
+  </si>
+  <si>
+    <t>int[][].clone()</t>
+  </si>
+  <si>
+    <t>int[0]</t>
+  </si>
+  <si>
+    <t>int[1]</t>
+  </si>
+  <si>
+    <t>int[2]</t>
+  </si>
+  <si>
+    <t>int[3]</t>
+  </si>
+  <si>
+    <t>int[][]</t>
+  </si>
+  <si>
+    <t>int[0][1]</t>
+  </si>
+  <si>
+    <t>int[0][2]</t>
+  </si>
+  <si>
+    <t>Integer[].clone()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int[].clone() </t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>[obj,obj]</t>
+  </si>
+  <si>
+    <t>[ref,ref]</t>
+  </si>
+  <si>
+    <t>&gt;deep</t>
+  </si>
+  <si>
+    <t>&gt;shallow</t>
+  </si>
+  <si>
+    <t>change the copy</t>
+  </si>
+  <si>
+    <t>ref = new Integer(10)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Change  reflected in original</t>
+  </si>
+  <si>
+    <t>Change  reflected in copy</t>
+  </si>
+  <si>
+    <t>int[0] = 5;</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>test (Integer[] ,int[] ).clone()</t>
+  </si>
+  <si>
+    <t>obj 1 = t1;</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test _cpy</t>
+  </si>
+  <si>
+    <t>obj 2 = t2;</t>
+  </si>
+  <si>
+    <t>test_cpy = test.clone ()</t>
+  </si>
+  <si>
+    <t>obj1_cpy = t1; // reference copied</t>
+  </si>
+  <si>
+    <t>obj2_cpy = t2; // reference copied</t>
+  </si>
+  <si>
+    <t>obj_cpy = obj1.clone()</t>
+  </si>
+  <si>
+    <t>class level clone</t>
+  </si>
+  <si>
+    <t>object level clone</t>
+  </si>
+  <si>
+    <t>class level clone + object level clone</t>
+  </si>
+  <si>
+    <t>obj1_cpy = t1; // values will get copied</t>
   </si>
 </sst>
 </file>
@@ -470,7 +636,7 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -521,7 +687,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -550,11 +716,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F79AC6D-F369-CE4B-8BB4-75AB025EC90A}" name="Table1" displayName="Table1" ref="A1:B27" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F79AC6D-F369-CE4B-8BB4-75AB025EC90A}" name="Table1" displayName="Table1" ref="A1:B27" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B27" xr:uid="{2F79AC6D-F369-CE4B-8BB4-75AB025EC90A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E50F22BA-054E-B347-86BC-2BE57D6675F8}" name="Method Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2209FEEC-7A7E-7F42-9945-21AAD078206A}" name="Function" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E50F22BA-054E-B347-86BC-2BE57D6675F8}" name="Method Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2209FEEC-7A7E-7F42-9945-21AAD078206A}" name="Function" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -856,25 +1022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677C165-95F6-4E48-AFD7-827BD620B4AF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33C0B6D-7EF4-7C47-A160-88CB5B4993C3}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A2:B27"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1109,4 +1261,309 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B36404-5F66-0541-B736-D2DF864FCD1C}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25E74E2-FB33-D642-B192-841055800CB3}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>